<commit_message>
Almost all is done
</commit_message>
<xml_diff>
--- a/Project/Результаты.xlsx
+++ b/Project/Результаты.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vadvergasov/workspace/ACS/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\ACS\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281132E-95F8-DE44-8B2D-9B744830FF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B1D8DE-0F1D-4804-A89B-5A31ACB9D884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" activeTab="2" xr2:uid="{399BC83B-FFB2-40CA-BF3D-628FC2C29C26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{399BC83B-FFB2-40CA-BF3D-628FC2C29C26}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -199,7 +199,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="54">
     <dxf>
@@ -380,7 +380,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -752,7 +752,7 @@
           </c:marker>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -941,7 +941,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043797727"/>
@@ -1006,7 +1006,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043796063"/>
@@ -1034,7 +1034,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1048,7 +1048,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1121,7 +1121,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2480,7 +2480,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -3191,7 +3191,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3228,7 +3228,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -3347,7 +3347,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3383,7 +3383,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -3427,7 +3427,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3457,7 +3457,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3471,7 +3471,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3542,7 +3542,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6101,7 +6101,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -7412,7 +7412,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7449,7 +7449,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -7568,7 +7568,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7604,7 +7604,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -7646,7 +7646,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7676,7 +7676,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7690,7 +7690,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7761,7 +7761,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9120,7 +9120,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -9831,7 +9831,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9868,7 +9868,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -9987,7 +9987,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10023,7 +10023,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -10066,7 +10066,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10096,7 +10096,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10110,7 +10110,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10181,7 +10181,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -11554,7 +11554,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11591,7 +11591,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -11712,7 +11712,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11748,7 +11748,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -11791,7 +11791,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -11821,7 +11821,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11835,7 +11835,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -11906,7 +11906,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13288,7 +13288,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13325,7 +13325,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -13446,7 +13446,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -13482,7 +13482,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -13525,7 +13525,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -13555,7 +13555,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -13569,7 +13569,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -14321,7 +14321,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14358,7 +14358,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -14452,7 +14452,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14488,7 +14488,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -14532,7 +14532,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14562,7 +14562,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14576,7 +14576,7 @@
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -15328,7 +15328,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15365,7 +15365,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -15459,7 +15459,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15495,7 +15495,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -15539,7 +15539,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -15569,7 +15569,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15583,7 +15583,7 @@
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -16335,7 +16335,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -16372,7 +16372,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -16466,7 +16466,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -16502,7 +16502,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -16546,7 +16546,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -16576,7 +16576,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16590,7 +16590,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -16653,7 +16653,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -17018,7 +17018,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -17207,7 +17207,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043797727"/>
@@ -17273,7 +17273,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043796063"/>
@@ -17315,7 +17315,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -17345,7 +17345,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -17359,7 +17359,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -17421,7 +17421,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -17459,7 +17459,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -17622,7 +17622,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -17811,7 +17811,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="976803295"/>
@@ -17876,7 +17876,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="976790815"/>
@@ -17918,7 +17918,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -17948,7 +17948,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -17962,7 +17962,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -18061,7 +18061,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -18274,7 +18274,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043797727"/>
@@ -18339,7 +18339,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1043796063"/>
@@ -18381,7 +18381,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -18411,7 +18411,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -18425,7 +18425,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -18488,7 +18488,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -19727,7 +19727,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -20348,7 +20348,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="957226943"/>
@@ -20413,7 +20413,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="957224447"/>
@@ -20456,7 +20456,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -20486,7 +20486,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -20500,7 +20500,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -20563,7 +20563,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -21792,7 +21792,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -22414,7 +22414,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1047549327"/>
@@ -22473,7 +22473,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1047549743"/>
@@ -22515,7 +22515,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -22545,7 +22545,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -22559,7 +22559,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -22626,7 +22626,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -23851,7 +23851,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1132622959"/>
@@ -23910,7 +23910,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1132640847"/>
@@ -23952,7 +23952,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -23982,7 +23982,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -23996,7 +23996,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -24067,7 +24067,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -25432,7 +25432,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -26146,7 +26146,7 @@
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -26183,7 +26183,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -26302,7 +26302,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -26338,7 +26338,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -26380,7 +26380,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -26410,7 +26410,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -26424,7 +26424,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -26500,7 +26500,7 @@
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -27214,7 +27214,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299346784"/>
@@ -27278,7 +27278,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="299348864"/>
@@ -27321,7 +27321,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -27351,7 +27351,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -37118,9 +37118,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -37158,7 +37158,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -37264,7 +37264,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -37420,47 +37420,47 @@
       <selection activeCell="Y2" sqref="Y2:AB202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -37516,7 +37516,7 @@
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -37626,7 +37626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -37736,7 +37736,7 @@
         <v>47200</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>150</v>
       </c>
@@ -37846,7 +37846,7 @@
         <v>59500</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>200</v>
       </c>
@@ -37956,7 +37956,7 @@
         <v>180700</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>250</v>
       </c>
@@ -38066,7 +38066,7 @@
         <v>339300</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>300</v>
       </c>
@@ -38176,7 +38176,7 @@
         <v>749000</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>350</v>
       </c>
@@ -38286,7 +38286,7 @@
         <v>1100700</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>400</v>
       </c>
@@ -38396,7 +38396,7 @@
         <v>1970600</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>450</v>
       </c>
@@ -38506,7 +38506,7 @@
         <v>3155100</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>500</v>
       </c>
@@ -38616,7 +38616,7 @@
         <v>4353500</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>550</v>
       </c>
@@ -38726,7 +38726,7 @@
         <v>5207000</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>600</v>
       </c>
@@ -38836,7 +38836,7 @@
         <v>8063500</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>650</v>
       </c>
@@ -38946,7 +38946,7 @@
         <v>8949700</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>700</v>
       </c>
@@ -39056,7 +39056,7 @@
         <v>13263200</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>750</v>
       </c>
@@ -39166,7 +39166,7 @@
         <v>14355100</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>800</v>
       </c>
@@ -39276,7 +39276,7 @@
         <v>19310000</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>850</v>
       </c>
@@ -39386,7 +39386,7 @@
         <v>24573900</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>900</v>
       </c>
@@ -39496,7 +39496,7 @@
         <v>25428000</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>950</v>
       </c>
@@ -39606,7 +39606,7 @@
         <v>19790200</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -39700,7 +39700,7 @@
         <v>25833900</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -39794,7 +39794,7 @@
         <v>28468000</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -39888,7 +39888,7 @@
         <v>37094300</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -39982,7 +39982,7 @@
         <v>37781200</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -40076,7 +40076,7 @@
         <v>48230700</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -40170,7 +40170,7 @@
         <v>57821100</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -40264,7 +40264,7 @@
         <v>61966300</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -40358,7 +40358,7 @@
         <v>63337100</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -40452,7 +40452,7 @@
         <v>79421200</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -40546,7 +40546,7 @@
         <v>77506600</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -40640,7 +40640,7 @@
         <v>99117600</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -40734,7 +40734,7 @@
         <v>97443600</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -40828,7 +40828,7 @@
         <v>121042300</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -40922,7 +40922,7 @@
         <v>137656100</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -41016,7 +41016,7 @@
         <v>145950100</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -41110,7 +41110,7 @@
         <v>143914500</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -41204,7 +41204,7 @@
         <v>175784200</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -41298,7 +41298,7 @@
         <v>167991000</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -41392,7 +41392,7 @@
         <v>207777700</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -41486,7 +41486,7 @@
         <v>201312300</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -41580,7 +41580,7 @@
         <v>241318500</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -41674,7 +41674,7 @@
         <v>269848000</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -41768,7 +41768,7 @@
         <v>274566900</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -41862,7 +41862,7 @@
         <v>271394800</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -41956,7 +41956,7 @@
         <v>327387800</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -42050,7 +42050,7 @@
         <v>308711300</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -42144,7 +42144,7 @@
         <v>381827700</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -42238,7 +42238,7 @@
         <v>359138400</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -42332,7 +42332,7 @@
         <v>435832300</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -42426,7 +42426,7 @@
         <v>470364400</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -42520,7 +42520,7 @@
         <v>496264500</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -42614,7 +42614,7 @@
         <v>466380300</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -42708,7 +42708,7 @@
         <v>566843400</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -42802,7 +42802,7 @@
         <v>512977600</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -42896,7 +42896,7 @@
         <v>631635700</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -42990,7 +42990,7 @@
         <v>585900000</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -43084,7 +43084,7 @@
         <v>714649800</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -43178,7 +43178,7 @@
         <v>753451400</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -43272,7 +43272,7 @@
         <v>792252000</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -43366,7 +43366,7 @@
         <v>729452200</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -43460,7 +43460,7 @@
         <v>886381100</v>
       </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -43554,7 +43554,7 @@
         <v>792718700</v>
       </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -43648,7 +43648,7 @@
         <v>976047800</v>
       </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -43742,7 +43742,7 @@
         <v>898349400</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -43836,7 +43836,7 @@
         <v>1089309500</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -43930,7 +43930,7 @@
         <v>1131293100</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -44024,7 +44024,7 @@
         <v>1196202200</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -44118,7 +44118,7 @@
         <v>1094641400</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -44212,7 +44212,7 @@
         <v>1321327700</v>
       </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -44306,7 +44306,7 @@
         <v>1178462200</v>
       </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -44400,7 +44400,7 @@
         <v>1441607100</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -44494,7 +44494,7 @@
         <v>1305316400</v>
       </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -44588,7 +44588,7 @@
         <v>1572638700</v>
       </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -44682,7 +44682,7 @@
         <v>1618462600</v>
       </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -44776,7 +44776,7 @@
         <v>1724269500</v>
       </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -44870,7 +44870,7 @@
         <v>1554061600</v>
       </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -44964,7 +44964,7 @@
         <v>1878473100</v>
       </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -45058,7 +45058,7 @@
         <v>1656120300</v>
       </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -45152,7 +45152,7 @@
         <v>2031459500</v>
       </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -45246,7 +45246,7 @@
         <v>1811854200</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -45340,7 +45340,7 @@
         <v>2198072800</v>
       </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -45434,7 +45434,7 @@
         <v>2237531100</v>
       </c>
     </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -45528,7 +45528,7 @@
         <v>2346310300</v>
       </c>
     </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -45622,7 +45622,7 @@
         <v>2081203700</v>
       </c>
     </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -45716,7 +45716,7 @@
         <v>2555721700</v>
       </c>
     </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -45810,7 +45810,7 @@
         <v>2257308200</v>
       </c>
     </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -45904,7 +45904,7 @@
         <v>2748480200</v>
       </c>
     </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -45998,7 +45998,7 @@
         <v>2496623500</v>
       </c>
     </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -46092,7 +46092,7 @@
         <v>3010164200</v>
       </c>
     </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -46186,7 +46186,7 @@
         <v>2995417500</v>
       </c>
     </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -46280,7 +46280,7 @@
         <v>3172186400</v>
       </c>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -46374,7 +46374,7 @@
         <v>2875806300</v>
       </c>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -46452,7 +46452,7 @@
         <v>3418138800</v>
       </c>
     </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -46530,7 +46530,7 @@
         <v>4520189900</v>
       </c>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -46608,7 +46608,7 @@
         <v>3671197100</v>
       </c>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -46686,7 +46686,7 @@
         <v>3369169900</v>
       </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -46764,7 +46764,7 @@
         <v>3957784000</v>
       </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -46842,7 +46842,7 @@
         <v>3915041700</v>
       </c>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -46920,7 +46920,7 @@
         <v>4240580100</v>
       </c>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -46998,7 +46998,7 @@
         <v>5519398100</v>
       </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -47076,7 +47076,7 @@
         <v>4531197100</v>
       </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -47154,7 +47154,7 @@
         <v>6190348100</v>
       </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y103" s="1">
         <v>10100</v>
       </c>
@@ -47168,7 +47168,7 @@
         <v>7168659200</v>
       </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y104" s="1">
         <v>10200</v>
       </c>
@@ -47182,7 +47182,7 @@
         <v>6807713000</v>
       </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y105" s="1">
         <v>10300</v>
       </c>
@@ -47196,7 +47196,7 @@
         <v>5220762500</v>
       </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y106" s="1">
         <v>10400</v>
       </c>
@@ -47210,7 +47210,7 @@
         <v>5021895100</v>
       </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y107" s="1">
         <v>10500</v>
       </c>
@@ -47224,7 +47224,7 @@
         <v>5573705900</v>
       </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y108" s="1">
         <v>10600</v>
       </c>
@@ -47238,7 +47238,7 @@
         <v>7988271700</v>
       </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y109" s="1">
         <v>10700</v>
       </c>
@@ -47252,7 +47252,7 @@
         <v>6000266300</v>
       </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y110" s="1">
         <v>10800</v>
       </c>
@@ -47266,7 +47266,7 @@
         <v>8660593300</v>
       </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y111" s="1">
         <v>10900</v>
       </c>
@@ -47280,7 +47280,7 @@
         <v>6317493300</v>
       </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="Y112" s="1">
         <v>11000</v>
       </c>
@@ -47294,7 +47294,7 @@
         <v>9296156000</v>
       </c>
     </row>
-    <row r="113" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="113" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y113" s="1">
         <v>11100</v>
       </c>
@@ -47308,7 +47308,7 @@
         <v>7354397800</v>
       </c>
     </row>
-    <row r="114" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="114" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y114" s="1">
         <v>11200</v>
       </c>
@@ -47322,7 +47322,7 @@
         <v>6300431900</v>
       </c>
     </row>
-    <row r="115" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="115" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y115" s="1">
         <v>11300</v>
       </c>
@@ -47336,7 +47336,7 @@
         <v>7696143600</v>
       </c>
     </row>
-    <row r="116" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="116" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y116" s="1">
         <v>11400</v>
       </c>
@@ -47350,7 +47350,7 @@
         <v>10361701100</v>
       </c>
     </row>
-    <row r="117" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="117" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y117" s="1">
         <v>11500</v>
       </c>
@@ -47364,7 +47364,7 @@
         <v>8316801700</v>
       </c>
     </row>
-    <row r="118" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="118" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y118" s="1">
         <v>11600</v>
       </c>
@@ -47378,7 +47378,7 @@
         <v>10754115900</v>
       </c>
     </row>
-    <row r="119" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="119" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y119" s="1">
         <v>11700</v>
       </c>
@@ -47392,7 +47392,7 @@
         <v>9296709000</v>
       </c>
     </row>
-    <row r="120" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="120" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y120" s="1">
         <v>11800</v>
       </c>
@@ -47406,7 +47406,7 @@
         <v>11549398500</v>
       </c>
     </row>
-    <row r="121" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="121" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y121" s="1">
         <v>11900</v>
       </c>
@@ -47420,7 +47420,7 @@
         <v>10198840400</v>
       </c>
     </row>
-    <row r="122" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="122" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y122" s="1">
         <v>12000</v>
       </c>
@@ -47434,7 +47434,7 @@
         <v>8038960100</v>
       </c>
     </row>
-    <row r="123" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="123" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y123" s="1">
         <v>12100</v>
       </c>
@@ -47448,7 +47448,7 @@
         <v>10899253000</v>
       </c>
     </row>
-    <row r="124" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="124" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y124" s="1">
         <v>12200</v>
       </c>
@@ -47462,7 +47462,7 @@
         <v>13827617000</v>
       </c>
     </row>
-    <row r="125" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="125" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y125" s="1">
         <v>12300</v>
       </c>
@@ -47476,7 +47476,7 @@
         <v>13217014200</v>
       </c>
     </row>
-    <row r="126" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="126" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y126" s="1">
         <v>12400</v>
       </c>
@@ -47490,7 +47490,7 @@
         <v>13884708000</v>
       </c>
     </row>
-    <row r="127" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y127" s="1">
         <v>12500</v>
       </c>
@@ -47504,7 +47504,7 @@
         <v>12301603600</v>
       </c>
     </row>
-    <row r="128" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="128" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y128" s="1">
         <v>12600</v>
       </c>
@@ -47518,7 +47518,7 @@
         <v>14846397000</v>
       </c>
     </row>
-    <row r="129" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="129" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y129" s="1">
         <v>12700</v>
       </c>
@@ -47532,7 +47532,7 @@
         <v>13766027100</v>
       </c>
     </row>
-    <row r="130" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="130" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y130" s="1">
         <v>12800</v>
       </c>
@@ -47546,7 +47546,7 @@
         <v>11685520700</v>
       </c>
     </row>
-    <row r="131" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="131" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y131" s="1">
         <v>12900</v>
       </c>
@@ -47560,7 +47560,7 @@
         <v>14767429200</v>
       </c>
     </row>
-    <row r="132" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="132" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y132" s="1">
         <v>13000</v>
       </c>
@@ -47574,7 +47574,7 @@
         <v>18595671100</v>
       </c>
     </row>
-    <row r="133" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="133" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y133" s="1">
         <v>13100</v>
       </c>
@@ -47588,7 +47588,7 @@
         <v>15856786700</v>
       </c>
     </row>
-    <row r="134" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="134" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y134" s="1">
         <v>13200</v>
       </c>
@@ -47602,7 +47602,7 @@
         <v>17622611800</v>
       </c>
     </row>
-    <row r="135" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="135" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y135" s="1">
         <v>13300</v>
       </c>
@@ -47616,7 +47616,7 @@
         <v>16090161200</v>
       </c>
     </row>
-    <row r="136" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="136" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y136" s="1">
         <v>13400</v>
       </c>
@@ -47630,7 +47630,7 @@
         <v>20253420900</v>
       </c>
     </row>
-    <row r="137" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="137" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y137" s="1">
         <v>13500</v>
       </c>
@@ -47644,7 +47644,7 @@
         <v>17949088800</v>
       </c>
     </row>
-    <row r="138" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="138" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y138" s="1">
         <v>13600</v>
       </c>
@@ -47658,7 +47658,7 @@
         <v>18601060500</v>
       </c>
     </row>
-    <row r="139" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="139" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y139" s="1">
         <v>13700</v>
       </c>
@@ -47672,7 +47672,7 @@
         <v>18885847700</v>
       </c>
     </row>
-    <row r="140" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="140" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y140" s="1">
         <v>13800</v>
       </c>
@@ -47686,7 +47686,7 @@
         <v>21166469700</v>
       </c>
     </row>
-    <row r="141" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="141" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y141" s="1">
         <v>13900</v>
       </c>
@@ -47700,7 +47700,7 @@
         <v>21000451500</v>
       </c>
     </row>
-    <row r="142" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="142" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y142" s="1">
         <v>14000</v>
       </c>
@@ -47714,7 +47714,7 @@
         <v>21081898500</v>
       </c>
     </row>
-    <row r="143" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="143" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y143" s="1">
         <v>14100</v>
       </c>
@@ -47728,7 +47728,7 @@
         <v>21376747900</v>
       </c>
     </row>
-    <row r="144" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="144" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y144" s="1">
         <v>14200</v>
       </c>
@@ -47742,7 +47742,7 @@
         <v>23600780400</v>
       </c>
     </row>
-    <row r="145" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="145" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y145" s="1">
         <v>14300</v>
       </c>
@@ -47756,7 +47756,7 @@
         <v>22492407500</v>
       </c>
     </row>
-    <row r="146" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="146" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y146" s="1">
         <v>14400</v>
       </c>
@@ -47770,7 +47770,7 @@
         <v>23520096700</v>
       </c>
     </row>
-    <row r="147" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="147" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y147" s="1">
         <v>14500</v>
       </c>
@@ -47784,7 +47784,7 @@
         <v>24094664700</v>
       </c>
     </row>
-    <row r="148" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="148" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y148" s="1">
         <v>14600</v>
       </c>
@@ -47798,7 +47798,7 @@
         <v>25992474100</v>
       </c>
     </row>
-    <row r="149" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="149" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y149" s="1">
         <v>14700</v>
       </c>
@@ -47812,7 +47812,7 @@
         <v>25525197400</v>
       </c>
     </row>
-    <row r="150" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="150" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y150" s="1">
         <v>14800</v>
       </c>
@@ -47826,7 +47826,7 @@
         <v>26818156000</v>
       </c>
     </row>
-    <row r="151" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="151" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y151" s="1">
         <v>14900</v>
       </c>
@@ -47840,7 +47840,7 @@
         <v>29876575000</v>
       </c>
     </row>
-    <row r="152" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="152" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y152" s="1">
         <v>15000</v>
       </c>
@@ -47854,7 +47854,7 @@
         <v>28829077300</v>
       </c>
     </row>
-    <row r="153" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="153" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y153" s="1">
         <v>15100</v>
       </c>
@@ -47868,7 +47868,7 @@
         <v>28496336600</v>
       </c>
     </row>
-    <row r="154" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="154" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y154" s="1">
         <v>15200</v>
       </c>
@@ -47882,7 +47882,7 @@
         <v>27425657000</v>
       </c>
     </row>
-    <row r="155" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="155" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y155" s="1">
         <v>15300</v>
       </c>
@@ -47896,7 +47896,7 @@
         <v>31251082400</v>
       </c>
     </row>
-    <row r="156" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="156" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y156" s="1">
         <v>15400</v>
       </c>
@@ -47910,7 +47910,7 @@
         <v>32498587600</v>
       </c>
     </row>
-    <row r="157" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="157" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y157" s="1">
         <v>15500</v>
       </c>
@@ -47924,7 +47924,7 @@
         <v>31619444600</v>
       </c>
     </row>
-    <row r="158" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="158" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y158" s="1">
         <v>15600</v>
       </c>
@@ -47938,7 +47938,7 @@
         <v>31568162700</v>
       </c>
     </row>
-    <row r="159" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="159" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y159" s="1">
         <v>15700</v>
       </c>
@@ -47952,7 +47952,7 @@
         <v>33351129100</v>
       </c>
     </row>
-    <row r="160" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="160" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y160" s="1">
         <v>15800</v>
       </c>
@@ -47966,7 +47966,7 @@
         <v>36628476100</v>
       </c>
     </row>
-    <row r="161" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="161" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y161" s="1">
         <v>15900</v>
       </c>
@@ -47980,7 +47980,7 @@
         <v>36033401600</v>
       </c>
     </row>
-    <row r="162" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="162" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y162" s="1">
         <v>16000</v>
       </c>
@@ -47994,7 +47994,7 @@
         <v>33026093500</v>
       </c>
     </row>
-    <row r="163" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="163" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y163" s="1">
         <v>16100</v>
       </c>
@@ -48008,7 +48008,7 @@
         <v>37037741200</v>
       </c>
     </row>
-    <row r="164" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="164" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y164" s="1">
         <v>16200</v>
       </c>
@@ -48022,7 +48022,7 @@
         <v>37781790100</v>
       </c>
     </row>
-    <row r="165" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="165" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y165" s="1">
         <v>16300</v>
       </c>
@@ -48036,7 +48036,7 @@
         <v>38234754300</v>
       </c>
     </row>
-    <row r="166" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="166" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y166" s="1">
         <v>16400</v>
       </c>
@@ -48050,7 +48050,7 @@
         <v>37180357400</v>
       </c>
     </row>
-    <row r="167" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="167" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y167" s="1">
         <v>16500</v>
       </c>
@@ -48064,7 +48064,7 @@
         <v>39585497700</v>
       </c>
     </row>
-    <row r="168" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="168" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y168" s="1">
         <v>16600</v>
       </c>
@@ -48078,7 +48078,7 @@
         <v>41176162000</v>
       </c>
     </row>
-    <row r="169" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="169" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y169" s="1">
         <v>16700</v>
       </c>
@@ -48092,7 +48092,7 @@
         <v>41932748100</v>
       </c>
     </row>
-    <row r="170" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="170" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y170" s="1">
         <v>16800</v>
       </c>
@@ -48106,7 +48106,7 @@
         <v>37764747100</v>
       </c>
     </row>
-    <row r="171" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="171" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y171" s="1">
         <v>16900</v>
       </c>
@@ -48120,7 +48120,7 @@
         <v>46182894100</v>
       </c>
     </row>
-    <row r="172" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="172" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y172" s="1">
         <v>17000</v>
       </c>
@@ -48134,7 +48134,7 @@
         <v>45175558100</v>
       </c>
     </row>
-    <row r="173" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="173" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y173" s="1">
         <v>17100</v>
       </c>
@@ -48148,7 +48148,7 @@
         <v>45345909100</v>
       </c>
     </row>
-    <row r="174" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="174" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y174" s="1">
         <v>17200</v>
       </c>
@@ -48162,7 +48162,7 @@
         <v>44226654400</v>
       </c>
     </row>
-    <row r="175" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="175" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y175" s="1">
         <v>17300</v>
       </c>
@@ -48176,7 +48176,7 @@
         <v>48993716600</v>
       </c>
     </row>
-    <row r="176" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="176" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y176" s="1">
         <v>17400</v>
       </c>
@@ -48190,7 +48190,7 @@
         <v>51559116300</v>
       </c>
     </row>
-    <row r="177" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="177" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y177" s="1">
         <v>17500</v>
       </c>
@@ -48204,7 +48204,7 @@
         <v>51433793800</v>
       </c>
     </row>
-    <row r="178" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="178" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y178" s="1">
         <v>17600</v>
       </c>
@@ -48218,7 +48218,7 @@
         <v>46678410800</v>
       </c>
     </row>
-    <row r="179" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="179" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y179" s="1">
         <v>17700</v>
       </c>
@@ -48232,7 +48232,7 @@
         <v>53430075900</v>
       </c>
     </row>
-    <row r="180" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="180" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y180" s="1">
         <v>17800</v>
       </c>
@@ -48246,7 +48246,7 @@
         <v>52503252100</v>
       </c>
     </row>
-    <row r="181" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="181" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y181" s="1">
         <v>17900</v>
       </c>
@@ -48260,7 +48260,7 @@
         <v>54301561700</v>
       </c>
     </row>
-    <row r="182" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="182" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y182" s="1">
         <v>18000</v>
       </c>
@@ -48274,7 +48274,7 @@
         <v>50929541600</v>
       </c>
     </row>
-    <row r="183" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="183" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y183" s="1">
         <v>18100</v>
       </c>
@@ -48288,7 +48288,7 @@
         <v>58964484900</v>
       </c>
     </row>
-    <row r="184" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="184" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y184" s="1">
         <v>18200</v>
       </c>
@@ -48302,7 +48302,7 @@
         <v>60569688000</v>
       </c>
     </row>
-    <row r="185" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="185" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y185" s="1">
         <v>18300</v>
       </c>
@@ -48316,7 +48316,7 @@
         <v>66082144000</v>
       </c>
     </row>
-    <row r="186" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="186" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y186" s="1">
         <v>18400</v>
       </c>
@@ -48330,7 +48330,7 @@
         <v>55292830800</v>
       </c>
     </row>
-    <row r="187" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="187" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y187" s="1">
         <v>18500</v>
       </c>
@@ -48344,7 +48344,7 @@
         <v>63354259000</v>
       </c>
     </row>
-    <row r="188" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="188" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y188" s="1">
         <v>18600</v>
       </c>
@@ -48358,7 +48358,7 @@
         <v>61775352400</v>
       </c>
     </row>
-    <row r="189" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="189" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y189" s="1">
         <v>18700</v>
       </c>
@@ -48372,7 +48372,7 @@
         <v>64190222800</v>
       </c>
     </row>
-    <row r="190" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="190" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y190" s="1">
         <v>18800</v>
       </c>
@@ -48386,7 +48386,7 @@
         <v>59542457600</v>
       </c>
     </row>
-    <row r="191" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="191" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y191" s="1">
         <v>18900</v>
       </c>
@@ -48400,7 +48400,7 @@
         <v>69237732400</v>
       </c>
     </row>
-    <row r="192" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="192" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y192" s="1">
         <v>19000</v>
       </c>
@@ -48414,7 +48414,7 @@
         <v>66935460300</v>
       </c>
     </row>
-    <row r="193" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="193" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y193" s="1">
         <v>19100</v>
       </c>
@@ -48428,7 +48428,7 @@
         <v>70511301500</v>
       </c>
     </row>
-    <row r="194" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="194" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y194" s="1">
         <v>19200</v>
       </c>
@@ -48442,7 +48442,7 @@
         <v>62490885100</v>
       </c>
     </row>
-    <row r="195" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="195" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y195" s="1">
         <v>19300</v>
       </c>
@@ -48456,7 +48456,7 @@
         <v>75217538000</v>
       </c>
     </row>
-    <row r="196" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="196" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y196" s="1">
         <v>19400</v>
       </c>
@@ -48470,7 +48470,7 @@
         <v>73521908500</v>
       </c>
     </row>
-    <row r="197" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="197" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y197" s="1">
         <v>19500</v>
       </c>
@@ -48484,7 +48484,7 @@
         <v>77490945600</v>
       </c>
     </row>
-    <row r="198" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="198" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y198" s="1">
         <v>19600</v>
       </c>
@@ -48498,7 +48498,7 @@
         <v>68392564300</v>
       </c>
     </row>
-    <row r="199" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="199" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y199" s="1">
         <v>19700</v>
       </c>
@@ -48512,7 +48512,7 @@
         <v>81515268700</v>
       </c>
     </row>
-    <row r="200" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="200" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y200" s="1">
         <v>19800</v>
       </c>
@@ -48526,7 +48526,7 @@
         <v>77158595000</v>
       </c>
     </row>
-    <row r="201" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="201" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y201" s="1">
         <v>19900</v>
       </c>
@@ -48540,7 +48540,7 @@
         <v>85025599500</v>
       </c>
     </row>
-    <row r="202" spans="25:28" x14ac:dyDescent="0.2">
+    <row r="202" spans="25:28" x14ac:dyDescent="0.25">
       <c r="Y202" s="1">
         <v>20000</v>
       </c>
@@ -48586,11 +48586,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05425C90-03A9-45DD-8249-DF023E7A352F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D90" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR169" sqref="AR169"/>
+    <sheetView tabSelected="1" topLeftCell="M4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL22" sqref="AL22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -48602,20 +48602,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6865BE7-0442-4D71-A95A-8F7ABA10D8EC}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -48632,7 +48632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" cm="1">
         <f t="array" ref="A2:A19">cpu_onethread[calculation_time]/cpu[calculation_time]</f>
         <v>1.766244550550135</v>
@@ -48654,7 +48654,7 @@
         <v>0.89393939393939392</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.5046169317974036</v>
       </c>
@@ -48671,7 +48671,7 @@
         <v>1.0033726812816188</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.9595940541764127</v>
       </c>
@@ -48688,7 +48688,7 @@
         <v>0.96424759871931698</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5.065326046792042</v>
       </c>
@@ -48705,7 +48705,7 @@
         <v>1.0050355450236967</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5.1830658292626195</v>
       </c>
@@ -48722,7 +48722,7 @@
         <v>1.0080753701211305</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5.3337751252833092</v>
       </c>
@@ -48739,7 +48739,7 @@
         <v>1.0019115237575096</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.0736558708899913</v>
       </c>
@@ -48756,7 +48756,7 @@
         <v>1.0007617693362449</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4.6007125020398991</v>
       </c>
@@ -48773,7 +48773,7 @@
         <v>1.0034347867569888</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5.8154658388611633</v>
       </c>
@@ -48790,7 +48790,7 @@
         <v>0.99811999908292637</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5.3061831755039446</v>
       </c>
@@ -48807,7 +48807,7 @@
         <v>1.001577287066246</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5.6255356069565892</v>
       </c>
@@ -48824,7 +48824,7 @@
         <v>1.0012541286909877</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.7589382855401601</v>
       </c>
@@ -48841,7 +48841,7 @@
         <v>1.0025203871314634</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5.6384710455435219</v>
       </c>
@@ -48858,7 +48858,7 @@
         <v>1.0008904719501335</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5.9927106031072102</v>
       </c>
@@ -48875,7 +48875,7 @@
         <v>1.0003693431267335</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5.5217331525935949</v>
       </c>
@@ -48892,7 +48892,7 @@
         <v>1.0007151667167629</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5.5349788659471715</v>
       </c>
@@ -48909,7 +48909,7 @@
         <v>1.0010428420705304</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5.4712241354779731</v>
       </c>
@@ -48926,7 +48926,7 @@
         <v>0.89789086748800306</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5.9946747067045481</v>
       </c>
@@ -48943,7 +48943,7 @@
         <v>0.89571923853318969</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>28.453201945543483</v>
       </c>
@@ -48957,7 +48957,7 @@
         <v>0.93040819413531561</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>24.911627510322916</v>
       </c>
@@ -48971,7 +48971,7 @@
         <v>0.97876948995203794</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>26.911211801549044</v>
       </c>
@@ -48985,7 +48985,7 @@
         <v>0.95873696072451331</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>24.289541247053105</v>
       </c>
@@ -48999,7 +48999,7 @@
         <v>0.96377416055079801</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>22.9046199874997</v>
       </c>
@@ -49013,7 +49013,7 @@
         <v>0.95484970689726856</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>23.997728216936924</v>
       </c>
@@ -49027,7 +49027,7 @@
         <v>0.96185107062534103</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>27.447611574354394</v>
       </c>
@@ -49041,7 +49041,7 @@
         <v>0.95501439465394267</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24.906693565455772</v>
       </c>
@@ -49055,7 +49055,7 @@
         <v>0.96289038448967057</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27.870137457302569</v>
       </c>
@@ -49069,7 +49069,7 @@
         <v>0.96533969914722728</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>24.697394848007328</v>
       </c>
@@ -49083,7 +49083,7 @@
         <v>0.9622542891160305</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27.608930650338312</v>
       </c>
@@ -49097,7 +49097,7 @@
         <v>0.96432626383601383</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>24.890491791358304</v>
       </c>
@@ -49111,7 +49111,7 @@
         <v>0.96373564315406046</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>24.154059494828413</v>
       </c>
@@ -49125,7 +49125,7 @@
         <v>0.95486939427215467</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>25.506880456952299</v>
       </c>
@@ -49139,7 +49139,7 @@
         <v>0.95603675907830055</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>27.276903618219698</v>
       </c>
@@ -49153,7 +49153,7 @@
         <v>0.95301343359502277</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>25.384473562954952</v>
       </c>
@@ -49167,7 +49167,7 @@
         <v>0.95905532905145052</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>28.709724122690655</v>
       </c>
@@ -49181,7 +49181,7 @@
         <v>0.960753149509469</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>24.686655834565016</v>
       </c>
@@ -49195,7 +49195,7 @@
         <v>0.96120087885931382</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>28.353953432365273</v>
       </c>
@@ -49209,7 +49209,7 @@
         <v>0.95488006191301666</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>25.30912467408529</v>
       </c>
@@ -49223,7 +49223,7 @@
         <v>0.96301769203686127</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>26.579919770826407</v>
       </c>
@@ -49237,7 +49237,7 @@
         <v>0.95652599585233289</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>28.617983691869792</v>
       </c>
@@ -49251,7 +49251,7 @@
         <v>0.96144945681355087</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>32.517808964664113</v>
       </c>
@@ -49265,7 +49265,7 @@
         <v>0.95415672923181816</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>28.381028866781161</v>
       </c>
@@ -49279,7 +49279,7 @@
         <v>0.95630275137871967</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>33.035894730938871</v>
       </c>
@@ -49293,7 +49293,7 @@
         <v>0.95944536481822462</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>25.307699002596301</v>
       </c>
@@ -49307,7 +49307,7 @@
         <v>0.95818975497684844</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>28.048603275014251</v>
       </c>
@@ -49321,7 +49321,7 @@
         <v>0.95901885774522344</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>24.286942025025773</v>
       </c>
@@ -49335,7 +49335,7 @@
         <v>0.96109982380382497</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>23.423244751342679</v>
       </c>
@@ -49349,7 +49349,7 @@
         <v>0.95206267507163422</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>21.778101963497182</v>
       </c>
@@ -49363,7 +49363,7 @@
         <v>0.95831854523406212</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>25.479332741764306</v>
       </c>
@@ -49377,7 +49377,7 @@
         <v>0.95433058237752422</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>23.117921516278912</v>
       </c>
@@ -49391,7 +49391,7 @@
         <v>0.96045987871828387</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>26.295229432389746</v>
       </c>
@@ -49405,7 +49405,7 @@
         <v>0.95758484104514718</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>24.956475529722002</v>
       </c>
@@ -49419,7 +49419,7 @@
         <v>0.96188770736335627</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>26.940869510559455</v>
       </c>
@@ -49433,7 +49433,7 @@
         <v>0.95238796729736441</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>24.274007825697993</v>
       </c>
@@ -49447,7 +49447,7 @@
         <v>0.96456924303292579</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>23.706776893268945</v>
       </c>
@@ -49461,7 +49461,7 @@
         <v>0.96129968991972781</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>23.518971579365672</v>
       </c>
@@ -49475,7 +49475,7 @@
         <v>0.96619385727799922</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>25.47651428453673</v>
       </c>
@@ -49489,7 +49489,7 @@
         <v>0.95860622334421985</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>23.326282265528363</v>
       </c>
@@ -49503,7 +49503,7 @@
         <v>0.96490696404239307</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>27.568781487186151</v>
       </c>
@@ -49517,7 +49517,7 @@
         <v>0.95758687715013302</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>22.378054492593066</v>
       </c>
@@ -49531,7 +49531,7 @@
         <v>0.96264603743945354</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>27.239861123955745</v>
       </c>
@@ -49545,7 +49545,7 @@
         <v>0.95956591206795594</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>22.989216499271706</v>
       </c>
@@ -49559,7 +49559,7 @@
         <v>0.96511374942349359</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>24.180407640994542</v>
       </c>
@@ -49573,7 +49573,7 @@
         <v>0.95973771098428862</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>23.6683388699477</v>
       </c>
@@ -49587,7 +49587,7 @@
         <v>0.96835870971342553</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>27.12564071172002</v>
       </c>
@@ -49601,7 +49601,7 @@
         <v>0.96638392596746869</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>23.335625214762519</v>
       </c>
@@ -49615,7 +49615,7 @@
         <v>0.96759561230636781</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>27.474384432830306</v>
       </c>
@@ -49629,7 +49629,7 @@
         <v>0.96683262160831829</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>23.294284975420656</v>
       </c>
@@ -49643,7 +49643,7 @@
         <v>0.9694347212228448</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>27.11356031665937</v>
       </c>
@@ -49657,7 +49657,7 @@
         <v>0.96540290539573592</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>23.202514730436931</v>
       </c>
@@ -49671,7 +49671,7 @@
         <v>0.97071104192432922</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>23.691520929518095</v>
       </c>
@@ -49685,7 +49685,7 @@
         <v>0.96685364694541154</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>23.408689142920114</v>
       </c>
@@ -49699,7 +49699,7 @@
         <v>0.97508778402761465</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>27.000612345511222</v>
       </c>
@@ -49713,7 +49713,7 @@
         <v>0.97359898192370253</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>24.377696867810091</v>
       </c>
@@ -49727,7 +49727,7 @@
         <v>0.97661698329944324</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>28.47247833241909</v>
       </c>
@@ -49741,7 +49741,7 @@
         <v>0.9744589030013816</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>24.346110293331446</v>
       </c>
@@ -49755,7 +49755,7 @@
         <v>0.9750750991740077</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>27.480759052501423</v>
       </c>
@@ -49769,7 +49769,7 @@
         <v>0.97600680965095155</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>23.412308121964895</v>
       </c>
@@ -49783,7 +49783,7 @@
         <v>0.97751523255297024</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>24.885798919308879</v>
       </c>
@@ -49797,7 +49797,7 @@
         <v>0.97793273113417578</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>23.209668328133713</v>
       </c>
@@ -49811,7 +49811,7 @@
         <v>0.98116612571363226</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>26.209973476118133</v>
       </c>
@@ -49825,7 +49825,7 @@
         <v>0.97894201211566323</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>22.806968393394971</v>
       </c>
@@ -49839,7 +49839,7 @@
         <v>0.97966303737272276</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>18.05533296262907</v>
       </c>
@@ -49853,7 +49853,7 @@
         <v>0.98072346208521211</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>22.772139436559279</v>
       </c>
@@ -49867,7 +49867,7 @@
         <v>0.98190731529819786</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>26.099469820376736</v>
       </c>
@@ -49881,7 +49881,7 @@
         <v>0.97995252624382401</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>22.512648739634162</v>
       </c>
@@ -49895,7 +49895,7 @@
         <v>0.98776599669521281</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>23.596882715566196</v>
       </c>
@@ -49909,7 +49909,7 @@
         <v>0.98393694517645502</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>22.200503869332575</v>
       </c>
@@ -49923,7 +49923,7 @@
         <v>0.98421470646199516</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>17.429440827817917</v>
       </c>
@@ -49937,7 +49937,7 @@
         <v>0.98440953871547998</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>23.395243829757607</v>
       </c>
@@ -49951,7 +49951,7 @@
         <v>0.98661374136058744</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>7.436775596012323</v>
       </c>
@@ -49962,7 +49962,7 @@
         <v>0.98453005475671584</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>7.4359120877285205</v>
       </c>
@@ -49973,7 +49973,7 @@
         <v>1.0095208782927201</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>7.2716597117808277</v>
       </c>
@@ -49984,7 +49984,7 @@
         <v>0.98729924256349577</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>7.2556201189085474</v>
       </c>
@@ -49995,7 +49995,7 @@
         <v>1.0080530370127996</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>7.0322291544159707</v>
       </c>
@@ -50006,7 +50006,7 @@
         <v>0.99328968342345958</v>
       </c>
     </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>7.2359168572512047</v>
       </c>
@@ -50017,7 +50017,7 @@
         <v>0.98993248125539191</v>
       </c>
     </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>7.3230232147415171</v>
       </c>
@@ -50028,7 +50028,7 @@
         <v>0.99082050935647048</v>
       </c>
     </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>7.2397993797987867</v>
       </c>
@@ -50039,7 +50039,7 @@
         <v>1.0129018309609883</v>
       </c>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>7.3125755497913341</v>
       </c>
@@ -50050,7 +50050,7 @@
         <v>0.99708338839131627</v>
       </c>
     </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>7.2241434936445872</v>
       </c>
@@ -50061,7 +50061,7 @@
         <v>1.0076863424294511</v>
       </c>
     </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C102">
         <f>AVERAGE(_xlfn.ANCHORARRAY(C2))</f>
         <v>7.4148080350721122</v>

</xml_diff>